<commit_message>
merge de archivos por mala configuracion
</commit_message>
<xml_diff>
--- a/Proyectos/2015/12/P1363 - AECCON, XML, Daniela Atrip_MO/Calidad/No_conformidades.xlsx
+++ b/Proyectos/2015/12/P1363 - AECCON, XML, Daniela Atrip_MO/Calidad/No_conformidades.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
   </bookViews>
   <sheets>
-    <sheet name="No Conformidades" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="No Conformidades" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>REPORTE DE NO CONFORMIDADES P1363 - AECCON, XML, Daniela Atrip_MO</t>
   </si>
@@ -50,7 +49,7 @@
     <t>En proceso</t>
   </si>
   <si>
-    <t>Plan de riegos en recursos humanos donde dice &lt;Cliente&gt; cambiarlo por nombre de cliente e &lt;interno&gt; por SOS Software </t>
+    <t>Plan de riegos en recursos humanos donde dice &lt;Cliente&gt; cambiarlo por nombre de cliente e &lt;interno&gt; por SOS Software</t>
   </si>
   <si>
     <t>Plan de proyecto seccion de riegos agregar efecto  de riesgo</t>
@@ -69,17 +68,19 @@
   </si>
   <si>
     <t>Enviar correo de creacion de linea base</t>
+  </si>
+  <si>
+    <t>hecho</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -88,22 +89,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -111,7 +97,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -153,95 +139,68 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -300,36 +259,324 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.8582995951417"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.9959514170041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.2793522267206"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5668016194332"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.2874493927125"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="0" width="10.8542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.5708502024292"/>
+    <col min="1" max="1" width="2.85546875"/>
+    <col min="2" max="2" width="42"/>
+    <col min="3" max="3" width="18.7109375"/>
+    <col min="4" max="4" width="24.28515625"/>
+    <col min="5" max="5" width="16.5703125"/>
+    <col min="6" max="6" width="10.85546875"/>
+    <col min="7" max="7" width="27.28515625"/>
+    <col min="8" max="1023" width="10.85546875"/>
+    <col min="1024" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="15.6" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -340,7 +587,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -349,7 +596,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" ht="30">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -372,8 +619,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+    <row r="4" spans="1:8">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -382,7 +629,7 @@
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="5">
         <v>42373</v>
       </c>
       <c r="E4" s="5"/>
@@ -390,9 +637,12 @@
         <v>10</v>
       </c>
       <c r="G4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -401,7 +651,7 @@
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="5">
         <v>42373</v>
       </c>
       <c r="E5" s="5"/>
@@ -409,9 +659,12 @@
         <v>10</v>
       </c>
       <c r="G5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="3">
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -420,7 +673,7 @@
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="5">
         <v>42373</v>
       </c>
       <c r="E6" s="5"/>
@@ -428,9 +681,12 @@
         <v>10</v>
       </c>
       <c r="G6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -439,7 +695,7 @@
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="5">
         <v>42375</v>
       </c>
       <c r="E7" s="5"/>
@@ -448,8 +704,8 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+    <row r="8" spans="1:8">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -458,7 +714,7 @@
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="5">
         <v>42373</v>
       </c>
       <c r="E8" s="5"/>
@@ -466,9 +722,12 @@
         <v>10</v>
       </c>
       <c r="G8" s="4"/>
-    </row>
-    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -477,7 +736,7 @@
       <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="5">
         <v>42373</v>
       </c>
       <c r="E9" s="5"/>
@@ -485,9 +744,12 @@
         <v>10</v>
       </c>
       <c r="G9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -496,7 +758,7 @@
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="5" t="n">
+      <c r="D10" s="5">
         <v>42373</v>
       </c>
       <c r="E10" s="5"/>
@@ -504,9 +766,12 @@
         <v>10</v>
       </c>
       <c r="G10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -517,9 +782,12 @@
       <c r="E11" s="3"/>
       <c r="F11" s="6"/>
       <c r="G11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="3"/>
@@ -529,8 +797,8 @@
       <c r="F12" s="6"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+    <row r="13" spans="1:8">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="3"/>
@@ -540,8 +808,8 @@
       <c r="F13" s="6"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+    <row r="14" spans="1:8">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="3"/>
@@ -551,8 +819,8 @@
       <c r="F14" s="6"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+    <row r="15" spans="1:8">
+      <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" s="3"/>
@@ -562,8 +830,8 @@
       <c r="F15" s="6"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+    <row r="16" spans="1:8">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="3"/>
@@ -573,8 +841,8 @@
       <c r="F16" s="6"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+    <row r="17" spans="1:7">
+      <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" s="3"/>
@@ -584,8 +852,8 @@
       <c r="F17" s="6"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+    <row r="18" spans="1:7">
+      <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" s="3"/>
@@ -595,8 +863,8 @@
       <c r="F18" s="6"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
+    <row r="19" spans="1:7">
+      <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" s="3"/>
@@ -606,8 +874,8 @@
       <c r="F19" s="6"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+    <row r="20" spans="1:7">
+      <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20" s="3"/>
@@ -617,8 +885,8 @@
       <c r="F20" s="6"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
+    <row r="21" spans="1:7">
+      <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" s="3"/>
@@ -628,8 +896,8 @@
       <c r="F21" s="6"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
+    <row r="22" spans="1:7">
+      <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" s="3"/>
@@ -639,8 +907,8 @@
       <c r="F22" s="6"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
+    <row r="23" spans="1:7">
+      <c r="A23" s="3">
         <v>21</v>
       </c>
       <c r="B23" s="3"/>
@@ -650,8 +918,8 @@
       <c r="F23" s="6"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
+    <row r="24" spans="1:7">
+      <c r="A24" s="3">
         <v>22</v>
       </c>
       <c r="B24" s="3"/>
@@ -661,8 +929,8 @@
       <c r="F24" s="6"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
+    <row r="25" spans="1:7">
+      <c r="A25" s="3">
         <v>23</v>
       </c>
       <c r="B25" s="3"/>
@@ -672,8 +940,8 @@
       <c r="F25" s="6"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
+    <row r="26" spans="1:7">
+      <c r="A26" s="3">
         <v>24</v>
       </c>
       <c r="B26" s="3"/>
@@ -683,8 +951,8 @@
       <c r="F26" s="6"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
+    <row r="27" spans="1:7">
+      <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27" s="3"/>
@@ -699,17 +967,12 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F4:F27" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F27">
       <formula1>"En proceso,Cerrada,Cancelada,Rechazada"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="1.14375" bottom="1.14375" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="1.14375" bottom="1.14375" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>